<commit_message>
added hw lesson 9
</commit_message>
<xml_diff>
--- a/Lesson 7/ДЗ 7.xlsx
+++ b/Lesson 7/ДЗ 7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -99,9 +99,6 @@
     <t>spyker</t>
   </si>
   <si>
-    <t>1НФ</t>
-  </si>
-  <si>
     <t>2НФ</t>
   </si>
   <si>
@@ -337,6 +334,15 @@
   </si>
   <si>
     <t>34,50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>вычисляемое поле</t>
+  </si>
+  <si>
+    <t>0НФ</t>
   </si>
 </sst>
 </file>
@@ -770,7 +776,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:10">
@@ -879,7 +885,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>1</v>
@@ -888,13 +894,13 @@
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="J14" t="s">
         <v>30</v>
-      </c>
-      <c r="J14" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:10">
@@ -1025,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>3</v>
@@ -1143,68 +1149,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:G10"/>
+  <dimension ref="A3:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7">
+    <row r="3" spans="1:7">
       <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="28.8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="D10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1216,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1239,10 +1252,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -1256,10 +1269,10 @@
         <v>15</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="28.8">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1270,10 +1283,10 @@
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="28.8">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -1284,7 +1297,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:8">
@@ -1298,7 +1311,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -1315,13 +1328,13 @@
         <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H9" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -1335,7 +1348,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>20</v>
@@ -1355,13 +1368,13 @@
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:8">
@@ -1375,10 +1388,10 @@
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>20</v>
@@ -1395,7 +1408,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>20</v>
@@ -1406,22 +1419,22 @@
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H17" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -1438,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:8">
@@ -1455,7 +1468,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:8">
@@ -1472,7 +1485,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:8">
@@ -1489,7 +1502,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -1497,7 +1510,7 @@
         <v>5</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -1505,7 +1518,7 @@
         <v>6</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -1513,7 +1526,7 @@
         <v>7</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="2:8">
@@ -1521,16 +1534,16 @@
         <v>0</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:8">
@@ -1622,25 +1635,25 @@
   <sheetData>
     <row r="3" spans="2:8">
       <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -1648,16 +1661,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="2">
         <v>203000</v>
@@ -1668,16 +1681,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2">
         <v>1118</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="2">
         <v>150</v>
@@ -1688,16 +1701,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2">
         <v>14800</v>
@@ -1708,16 +1721,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="2">
         <v>10200</v>
@@ -1728,16 +1741,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G8" s="2">
         <v>82399</v>
@@ -1748,16 +1761,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" s="2">
         <v>22374</v>
@@ -1765,19 +1778,19 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="2:8">
@@ -1785,10 +1798,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>13</v>
@@ -1799,13 +1812,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2">
         <v>1118</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -1813,13 +1826,13 @@
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -1827,10 +1840,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>13</v>
@@ -1841,13 +1854,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="2:5">
@@ -1855,21 +1868,21 @@
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -1877,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -1885,7 +1898,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -1893,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -1901,7 +1914,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="2:5">
@@ -1910,13 +1923,13 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="2:5">
@@ -2008,7 +2021,7 @@
   <sheetData>
     <row r="4" spans="2:9">
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -2017,16 +2030,16 @@
         <v>2</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -2034,19 +2047,19 @@
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -2054,19 +2067,19 @@
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -2074,19 +2087,19 @@
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -2094,24 +2107,24 @@
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
@@ -2120,7 +2133,7 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -2128,10 +2141,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -2139,10 +2152,10 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="2:9">
@@ -2150,10 +2163,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -2161,73 +2174,73 @@
         <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -2235,7 +2248,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -2243,7 +2256,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -2251,7 +2264,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -2259,7 +2272,7 @@
         <v>19</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2269,9 +2282,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:F7"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2282,18 +2295,23 @@
     <col min="4" max="4" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:6">
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="3" spans="2:6">
       <c r="B3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -2304,7 +2322,7 @@
         <v>13.44</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="2:6">
@@ -2312,10 +2330,10 @@
         <v>24</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="2:6">
@@ -2326,7 +2344,7 @@
         <v>543.44000000000005</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -2334,10 +2352,53 @@
         <v>19</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="2">
+        <v>23</v>
+      </c>
+      <c r="C11" s="12">
+        <v>13.44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="2">
+        <v>24</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="2">
+        <v>25</v>
+      </c>
+      <c r="C13" s="12">
+        <v>543.44000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="2">
+        <v>19</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>